<commit_message>
Added changes to recognize and install dependencies if missing
</commit_message>
<xml_diff>
--- a/Schedules/Horario_1.xlsx
+++ b/Schedules/Horario_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,490 +473,420 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Administracion de Proyectos</t>
+          <t>Redes Inalambricas</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51396</v>
+        <v>49362</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TECUANHUEHUE - VERA PEDRO</t>
+          <t>LOPEZ - MUNOZ MAURO ALBERTO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>13:59</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1CCO4/203</t>
+          <t>1CCO4/301</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Administracion de Proyectos</t>
+          <t>Redes Inalambricas</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>51396</v>
+        <v>49362</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TECUANHUEHUE - VERA PEDRO</t>
+          <t>LOPEZ - MUNOZ MAURO ALBERTO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>14:59</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1CCO4/203</t>
+          <t>1CCO3/303</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ecuaciones Diferenciales</t>
+          <t>Redes Inalambricas</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45797</v>
+        <v>49362</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ESPÍNDOLA - POZOS ARMANDO</t>
+          <t>LOPEZ - MUNOZ MAURO ALBERTO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>14:59</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1CCO4/305</t>
+          <t>1CCO4/301</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ecuaciones Diferenciales</t>
+          <t>Tec.de Inteligencia Artificial</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45797</v>
+        <v>49245</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ESPÍNDOLA - POZOS ARMANDO</t>
+          <t>TECUANHUEHUE - VERA PEDRO</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1CCO4/305</t>
+          <t>1CCO3/114</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ecuaciones Diferenciales</t>
+          <t>Tec.de Inteligencia Artificial</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>45797</v>
+        <v>49245</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ESPÍNDOLA - POZOS ARMANDO</t>
+          <t>TECUANHUEHUE - VERA PEDRO</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>12:59</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1CCO4/305</t>
+          <t>1CCO3/114</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Estructuras de Datos</t>
+          <t>Tec.de Inteligencia Artificial</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>41443</v>
+        <v>49245</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SANTIAGO - DÍAZ MARÍA DEL CARMEN</t>
+          <t>TECUANHUEHUE - VERA PEDRO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>V</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>12:59</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1CCO1/002</t>
+          <t>1CCO5/202</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Estructuras de Datos</t>
+          <t>Teoria de Control</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>41443</v>
+        <v>49190</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SANTIAGO - DÍAZ MARÍA DEL CARMEN</t>
+          <t>HERNANDEZ - AMECA JOSE LUIS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>12:59</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1CCO1/002</t>
+          <t>1CCO3/310</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Estructuras de Datos</t>
+          <t>Teoria de Control</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>41443</v>
+        <v>49190</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SANTIAGO - DÍAZ MARÍA DEL CARMEN</t>
+          <t>HERNANDEZ - AMECA JOSE LUIS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>12:59</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1CCO3/109</t>
+          <t>1CCO3/310</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Circuitos Eléctricos</t>
+          <t>Teoria de Control</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>47977</v>
+        <v>49190</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RODRÍGUEZ - PEDROZA BERENICE</t>
+          <t>HERNANDEZ - AMECA JOSE LUIS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>J</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>12:59</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1CCO5/202</t>
+          <t>1CCO1/002</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Circuitos Eléctricos</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>47977</v>
+        <v>49971</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RODRÍGUEZ - PEDROZA BERENICE</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>L</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>10:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1CCO3/309</t>
+          <t>1CCO4/103</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Circuitos Eléctricos</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>47977</v>
+        <v>49971</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RODRÍGUEZ - PEDROZA BERENICE</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>08:59</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1CCO5/202</t>
+          <t>1CCO4/103</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Graficación</t>
+          <t>Vision y Animacion por Comput.</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42328</v>
+        <v>49971</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ORATO - RAMÍREZ JOSÉ MARTÍN</t>
+          <t>JUAREZ - PEREZ SILVESTRE</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>J</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>14:59</t>
+          <t>10:59</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1CCO3/104</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Graficación</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>42328</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>ORATO - RAMÍREZ JOSÉ MARTÍN</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>14:59</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>1CCO3/104</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Graficación</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>42328</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ORATO - RAMÍREZ JOSÉ MARTÍN</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>J</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>14:59</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>1CCO3/104</t>
+          <t>1CCO4/308</t>
         </is>
       </c>
     </row>

</xml_diff>